<commit_message>
Added 2 winrar files and was modified word and excel
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NMK\nmk-izvp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zerzor13\dir_for_git\web-prog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EECEBC88-2522-476D-AF25-43B9B26384F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC0459C-879D-4926-A22D-F975348F94F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5407CB4B-62E8-4971-B1DD-41A867E52758}"/>
+    <workbookView xWindow="4335" yWindow="2325" windowWidth="21600" windowHeight="11295" xr2:uid="{5407CB4B-62E8-4971-B1DD-41A867E52758}"/>
   </bookViews>
   <sheets>
     <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="177">
   <si>
     <t>№</t>
   </si>
@@ -562,48 +562,6 @@
   </si>
   <si>
     <t>[5,10]</t>
-  </si>
-  <si>
-    <t>61.  </t>
-  </si>
-  <si>
-    <t>Архітектура MVC у фреймворку Laravel</t>
-  </si>
-  <si>
-    <t> 18</t>
-  </si>
-  <si>
-    <t>62.  </t>
-  </si>
-  <si>
-    <t>Створення порожнього проекту на базі фреймворку Laravel</t>
-  </si>
-  <si>
-    <t>63.  </t>
-  </si>
-  <si>
-    <t>Створення моделей та міграцій</t>
-  </si>
-  <si>
-    <t>64.  </t>
-  </si>
-  <si>
-    <t>Створення шаблонів та контроллерів. Завершення проєкту</t>
-  </si>
-  <si>
-    <t>65.  </t>
-  </si>
-  <si>
-    <t>Створення власних пакетів</t>
-  </si>
-  <si>
-    <t>МК2</t>
-  </si>
-  <si>
-    <t>66.  </t>
-  </si>
-  <si>
-    <t>Разом:</t>
   </si>
 </sst>
 </file>
@@ -811,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -861,9 +819,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -888,11 +843,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -906,35 +879,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1252,32 +1201,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AB4ACD-37B1-4AC7-AF77-03DE915FAA9E}">
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="20.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="61.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="61.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="28" t="s">
+      <c r="B1" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="28" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="29"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="5" t="s">
         <v>13</v>
       </c>
@@ -1286,20 +1235,20 @@
       </c>
       <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="38" t="s">
+      <c r="C2" s="36"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="39"/>
+      <c r="G2" s="38"/>
       <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
@@ -1310,18 +1259,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="38" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="39"/>
+      <c r="G3" s="38"/>
       <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
@@ -1332,16 +1281,16 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="38" t="s">
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="39"/>
+      <c r="G4" s="38"/>
       <c r="H4" s="6" t="s">
         <v>16</v>
       </c>
@@ -1350,86 +1299,86 @@
       </c>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="38" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="39"/>
+      <c r="G5" s="38"/>
       <c r="H5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="38" t="s">
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="39"/>
+      <c r="G6" s="38"/>
       <c r="H6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="38" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="39"/>
+      <c r="G7" s="38"/>
       <c r="H7" s="7"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="11" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="36"/>
-      <c r="G8" s="37"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>1</v>
       </c>
-      <c r="B9" s="40">
-        <v>2</v>
-      </c>
-      <c r="C9" s="41"/>
+      <c r="B9" s="27">
+        <v>2</v>
+      </c>
+      <c r="C9" s="28"/>
       <c r="D9" s="14">
         <v>3</v>
       </c>
       <c r="E9" s="14">
         <v>4</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="27">
         <v>5</v>
       </c>
-      <c r="G9" s="41"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="14">
         <v>6</v>
       </c>
@@ -1440,7 +1389,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>25</v>
       </c>
@@ -1450,324 +1399,324 @@
       <c r="C10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-    </row>
-    <row r="11" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="21" t="s">
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="19">
-        <v>2</v>
-      </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="23" t="s">
+      <c r="D11" s="18">
+        <v>2</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="18">
         <v>1</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J11" s="19" t="s">
+      <c r="I11" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
+    <row r="12" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="21"/>
+      <c r="C12" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19">
-        <v>2</v>
-      </c>
-      <c r="F12" s="23" t="s">
+      <c r="D12" s="18"/>
+      <c r="E12" s="18">
+        <v>2</v>
+      </c>
+      <c r="F12" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="18">
         <v>1</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="19" t="s">
+      <c r="I12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="21" t="s">
+    <row r="13" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="19">
-        <v>2</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="23" t="s">
+      <c r="D13" s="18">
+        <v>2</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="18">
         <v>1</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J13" s="19" t="s">
+      <c r="I13" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="21" t="s">
+    <row r="14" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="21"/>
+      <c r="C14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="19">
-        <v>2</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="23" t="s">
+      <c r="D14" s="18">
+        <v>2</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="19">
-        <v>2</v>
-      </c>
-      <c r="H14" s="19" t="s">
+      <c r="G14" s="18">
+        <v>2</v>
+      </c>
+      <c r="H14" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J14" s="19" t="s">
+      <c r="I14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="21" t="s">
+    <row r="15" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22" t="s">
+      <c r="B15" s="21"/>
+      <c r="C15" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19">
-        <v>2</v>
-      </c>
-      <c r="F15" s="23" t="s">
+      <c r="D15" s="18"/>
+      <c r="E15" s="18">
+        <v>2</v>
+      </c>
+      <c r="F15" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="19">
-        <v>2</v>
-      </c>
-      <c r="H15" s="19" t="s">
+      <c r="G15" s="18">
+        <v>2</v>
+      </c>
+      <c r="H15" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="19" t="s">
+      <c r="I15" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
+    <row r="16" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22" t="s">
+      <c r="B16" s="21"/>
+      <c r="C16" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="19">
-        <v>2</v>
-      </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="23" t="s">
+      <c r="D16" s="18">
+        <v>2</v>
+      </c>
+      <c r="E16" s="18"/>
+      <c r="F16" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="19">
-        <v>2</v>
-      </c>
-      <c r="H16" s="19" t="s">
+      <c r="G16" s="18">
+        <v>2</v>
+      </c>
+      <c r="H16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="19" t="s">
+      <c r="I16" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
+    <row r="17" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22" t="s">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="19">
-        <v>2</v>
-      </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="23" t="s">
+      <c r="D17" s="18">
+        <v>2</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="18">
         <v>3</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" s="19" t="s">
+      <c r="I17" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="21" t="s">
+    <row r="18" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19">
-        <v>2</v>
-      </c>
-      <c r="F18" s="23" t="s">
+      <c r="D18" s="18"/>
+      <c r="E18" s="18">
+        <v>2</v>
+      </c>
+      <c r="F18" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="18">
         <v>3</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I18" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="19" t="s">
+      <c r="I18" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
+    <row r="19" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="19">
-        <v>2</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="23" t="s">
+      <c r="D19" s="18">
+        <v>2</v>
+      </c>
+      <c r="E19" s="18"/>
+      <c r="F19" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="18">
         <v>3</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I19" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J19" s="19" t="s">
+      <c r="I19" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="21" t="s">
+    <row r="20" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22" t="s">
+      <c r="B20" s="21"/>
+      <c r="C20" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="19">
-        <v>2</v>
-      </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="23" t="s">
+      <c r="D20" s="18">
+        <v>2</v>
+      </c>
+      <c r="E20" s="18"/>
+      <c r="F20" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="18">
         <v>4</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J20" s="19" t="s">
+      <c r="I20" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="21" t="s">
+    <row r="21" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22" t="s">
+      <c r="B21" s="21"/>
+      <c r="C21" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="19">
-        <v>2</v>
-      </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="23" t="s">
+      <c r="D21" s="18">
+        <v>2</v>
+      </c>
+      <c r="E21" s="18"/>
+      <c r="F21" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="18">
         <v>4</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J21" s="19" t="s">
+      <c r="I21" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="21" t="s">
+    <row r="22" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B22" s="16" t="s">
@@ -1776,1236 +1725,1236 @@
       <c r="C22" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-    </row>
-    <row r="23" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="21" t="s">
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+    </row>
+    <row r="23" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22" t="s">
+      <c r="B23" s="21"/>
+      <c r="C23" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="19">
-        <v>2</v>
-      </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="23" t="s">
+      <c r="D23" s="18">
+        <v>2</v>
+      </c>
+      <c r="E23" s="18"/>
+      <c r="F23" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="18">
         <v>5</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I23" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J23" s="19" t="s">
+      <c r="I23" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="21" t="s">
+    <row r="24" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22" t="s">
+      <c r="B24" s="21"/>
+      <c r="C24" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19">
-        <v>2</v>
-      </c>
-      <c r="F24" s="23" t="s">
+      <c r="D24" s="18"/>
+      <c r="E24" s="18">
+        <v>2</v>
+      </c>
+      <c r="F24" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="18">
         <v>4</v>
       </c>
-      <c r="H24" s="19" t="s">
+      <c r="H24" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I24" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J24" s="19" t="s">
+      <c r="I24" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" s="18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="21" t="s">
+    <row r="25" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22" t="s">
+      <c r="B25" s="21"/>
+      <c r="C25" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="19">
-        <v>2</v>
-      </c>
-      <c r="E25" s="19"/>
-      <c r="F25" s="23" t="s">
+      <c r="D25" s="18">
+        <v>2</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="F25" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="18">
         <v>5</v>
       </c>
-      <c r="H25" s="19" t="s">
+      <c r="H25" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I25" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J25" s="19" t="s">
+      <c r="I25" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="21" t="s">
+    <row r="26" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="24" t="s">
+      <c r="B26" s="21"/>
+      <c r="C26" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="19">
-        <v>2</v>
-      </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="23" t="s">
+      <c r="D26" s="18">
+        <v>2</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="18">
         <v>6</v>
       </c>
-      <c r="H26" s="19" t="s">
+      <c r="H26" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I26" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J26" s="19" t="s">
+      <c r="I26" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J26" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="21" t="s">
+    <row r="27" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22" t="s">
+      <c r="B27" s="21"/>
+      <c r="C27" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19">
-        <v>2</v>
-      </c>
-      <c r="F27" s="23" t="s">
+      <c r="D27" s="18"/>
+      <c r="E27" s="18">
+        <v>2</v>
+      </c>
+      <c r="F27" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="19">
+      <c r="G27" s="18">
         <v>5</v>
       </c>
-      <c r="H27" s="19" t="s">
+      <c r="H27" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I27" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J27" s="19" t="s">
+      <c r="I27" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="21" t="s">
+    <row r="28" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22" t="s">
+      <c r="B28" s="21"/>
+      <c r="C28" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19">
-        <v>2</v>
-      </c>
-      <c r="F28" s="23" t="s">
+      <c r="D28" s="18"/>
+      <c r="E28" s="18">
+        <v>2</v>
+      </c>
+      <c r="F28" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="18">
         <v>6</v>
       </c>
-      <c r="H28" s="19" t="s">
+      <c r="H28" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I28" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J28" s="19" t="s">
+      <c r="I28" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="21" t="s">
+    <row r="29" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22" t="s">
+      <c r="B29" s="21"/>
+      <c r="C29" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="19">
-        <v>2</v>
-      </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="23" t="s">
+      <c r="D29" s="18">
+        <v>2</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G29" s="19">
+      <c r="G29" s="18">
         <v>7</v>
       </c>
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I29" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J29" s="19" t="s">
+      <c r="I29" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J29" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="21" t="s">
+    <row r="30" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22" t="s">
+      <c r="B30" s="21"/>
+      <c r="C30" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="D30" s="19">
-        <v>2</v>
-      </c>
-      <c r="E30" s="19"/>
-      <c r="F30" s="23" t="s">
+      <c r="D30" s="18">
+        <v>2</v>
+      </c>
+      <c r="E30" s="18"/>
+      <c r="F30" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="18">
         <v>6</v>
       </c>
-      <c r="H30" s="19" t="s">
+      <c r="H30" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I30" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J30" s="19" t="s">
+      <c r="I30" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="21" t="s">
+    <row r="31" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22" t="s">
+      <c r="B31" s="21"/>
+      <c r="C31" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19">
-        <v>2</v>
-      </c>
-      <c r="F31" s="23" t="s">
+      <c r="D31" s="18"/>
+      <c r="E31" s="18">
+        <v>2</v>
+      </c>
+      <c r="F31" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G31" s="19">
+      <c r="G31" s="18">
         <v>7</v>
       </c>
-      <c r="H31" s="19" t="s">
+      <c r="H31" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I31" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J31" s="19" t="s">
+      <c r="I31" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J31" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="21" t="s">
+    <row r="32" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22" t="s">
+      <c r="B32" s="21"/>
+      <c r="C32" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D32" s="19">
-        <v>2</v>
-      </c>
-      <c r="E32" s="19"/>
-      <c r="F32" s="23" t="s">
+      <c r="D32" s="18">
+        <v>2</v>
+      </c>
+      <c r="E32" s="18"/>
+      <c r="F32" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G32" s="19">
+      <c r="G32" s="18">
         <v>8</v>
       </c>
-      <c r="H32" s="19" t="s">
+      <c r="H32" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I32" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J32" s="19" t="s">
+      <c r="I32" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J32" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="21" t="s">
+    <row r="33" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22" t="s">
+      <c r="B33" s="21"/>
+      <c r="C33" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="D33" s="19">
-        <v>2</v>
-      </c>
-      <c r="E33" s="19"/>
-      <c r="F33" s="23" t="s">
+      <c r="D33" s="18">
+        <v>2</v>
+      </c>
+      <c r="E33" s="18"/>
+      <c r="F33" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G33" s="19">
+      <c r="G33" s="18">
         <v>7</v>
       </c>
-      <c r="H33" s="19" t="s">
+      <c r="H33" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I33" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J33" s="19" t="s">
+      <c r="I33" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J33" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="21" t="s">
+    <row r="34" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22" t="s">
+      <c r="B34" s="21"/>
+      <c r="C34" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="19">
-        <v>2</v>
-      </c>
-      <c r="E34" s="19"/>
-      <c r="F34" s="23" t="s">
+      <c r="D34" s="18">
+        <v>2</v>
+      </c>
+      <c r="E34" s="18"/>
+      <c r="F34" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G34" s="19">
+      <c r="G34" s="18">
         <v>9</v>
       </c>
-      <c r="H34" s="19" t="s">
+      <c r="H34" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I34" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J34" s="19" t="s">
+      <c r="I34" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J34" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="21" t="s">
+    <row r="35" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22" t="s">
+      <c r="B35" s="21"/>
+      <c r="C35" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="19">
-        <v>2</v>
-      </c>
-      <c r="E35" s="19"/>
-      <c r="F35" s="23" t="s">
+      <c r="D35" s="18">
+        <v>2</v>
+      </c>
+      <c r="E35" s="18"/>
+      <c r="F35" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G35" s="19">
+      <c r="G35" s="18">
         <v>8</v>
       </c>
-      <c r="H35" s="19" t="s">
+      <c r="H35" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I35" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J35" s="19" t="s">
+      <c r="I35" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J35" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="21" t="s">
+    <row r="36" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22" t="s">
+      <c r="B36" s="21"/>
+      <c r="C36" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19">
-        <v>2</v>
-      </c>
-      <c r="F36" s="23" t="s">
+      <c r="D36" s="18"/>
+      <c r="E36" s="18">
+        <v>2</v>
+      </c>
+      <c r="F36" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G36" s="19" t="s">
+      <c r="G36" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="H36" s="19" t="s">
+      <c r="H36" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I36" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J36" s="19" t="s">
+      <c r="I36" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J36" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="21" t="s">
+    <row r="37" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22" t="s">
+      <c r="B37" s="21"/>
+      <c r="C37" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="19">
-        <v>2</v>
-      </c>
-      <c r="E37" s="19"/>
-      <c r="F37" s="23" t="s">
+      <c r="D37" s="18">
+        <v>2</v>
+      </c>
+      <c r="E37" s="18"/>
+      <c r="F37" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G37" s="19">
+      <c r="G37" s="18">
         <v>10</v>
       </c>
-      <c r="H37" s="19" t="s">
+      <c r="H37" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I37" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J37" s="19" t="s">
+      <c r="I37" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J37" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="21" t="s">
+    <row r="38" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19">
-        <v>2</v>
-      </c>
-      <c r="F38" s="23" t="s">
+      <c r="D38" s="18"/>
+      <c r="E38" s="18">
+        <v>2</v>
+      </c>
+      <c r="F38" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G38" s="19">
+      <c r="G38" s="18">
         <v>9</v>
       </c>
-      <c r="H38" s="19" t="s">
+      <c r="H38" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I38" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J38" s="19" t="s">
+      <c r="I38" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J38" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="21" t="s">
+    <row r="39" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22" t="s">
+      <c r="B39" s="21"/>
+      <c r="C39" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="D39" s="19">
-        <v>2</v>
-      </c>
-      <c r="E39" s="19"/>
-      <c r="F39" s="23" t="s">
+      <c r="D39" s="18">
+        <v>2</v>
+      </c>
+      <c r="E39" s="18"/>
+      <c r="F39" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G39" s="19">
+      <c r="G39" s="18">
         <v>11</v>
       </c>
-      <c r="H39" s="19" t="s">
+      <c r="H39" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I39" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J39" s="19" t="s">
+      <c r="I39" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J39" s="18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="21" t="s">
+    <row r="40" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22" t="s">
+      <c r="B40" s="21"/>
+      <c r="C40" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="19">
-        <v>2</v>
-      </c>
-      <c r="E40" s="19"/>
-      <c r="F40" s="23" t="s">
+      <c r="D40" s="18">
+        <v>2</v>
+      </c>
+      <c r="E40" s="18"/>
+      <c r="F40" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G40" s="19">
+      <c r="G40" s="18">
         <v>9</v>
       </c>
-      <c r="H40" s="19" t="s">
+      <c r="H40" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I40" s="19" t="s">
+      <c r="I40" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J40" s="19" t="s">
+      <c r="J40" s="18" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="21" t="s">
+    <row r="41" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22" t="s">
+      <c r="B41" s="21"/>
+      <c r="C41" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="D41" s="19">
-        <v>2</v>
-      </c>
-      <c r="E41" s="19"/>
-      <c r="F41" s="23" t="s">
+      <c r="D41" s="18">
+        <v>2</v>
+      </c>
+      <c r="E41" s="18"/>
+      <c r="F41" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G41" s="19">
+      <c r="G41" s="18">
         <v>12</v>
       </c>
-      <c r="H41" s="19" t="s">
+      <c r="H41" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I41" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J41" s="19" t="s">
+      <c r="I41" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J41" s="18" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="21" t="s">
+    <row r="42" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="21" t="s">
         <v>110</v>
       </c>
       <c r="C42" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-    </row>
-    <row r="43" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="21" t="s">
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+    </row>
+    <row r="43" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22" t="s">
+      <c r="B43" s="21"/>
+      <c r="C43" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="D43" s="19">
-        <v>2</v>
-      </c>
-      <c r="E43" s="19"/>
-      <c r="F43" s="23" t="s">
+      <c r="D43" s="18">
+        <v>2</v>
+      </c>
+      <c r="E43" s="18"/>
+      <c r="F43" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G43" s="19">
+      <c r="G43" s="18">
         <v>10</v>
       </c>
-      <c r="H43" s="19" t="s">
+      <c r="H43" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I43" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J43" s="19" t="s">
+      <c r="I43" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J43" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="21" t="s">
+    <row r="44" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="B44" s="25"/>
-      <c r="C44" s="22" t="s">
+      <c r="B44" s="24"/>
+      <c r="C44" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19">
-        <v>2</v>
-      </c>
-      <c r="F44" s="23" t="s">
+      <c r="D44" s="18"/>
+      <c r="E44" s="18">
+        <v>2</v>
+      </c>
+      <c r="F44" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G44" s="19">
+      <c r="G44" s="18">
         <v>10</v>
       </c>
-      <c r="H44" s="19" t="s">
+      <c r="H44" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I44" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J44" s="19" t="s">
+      <c r="I44" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J44" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="21" t="s">
+    <row r="45" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="22" t="s">
+      <c r="B45" s="21"/>
+      <c r="C45" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="D45" s="19">
-        <v>2</v>
-      </c>
-      <c r="E45" s="19"/>
-      <c r="F45" s="23" t="s">
+      <c r="D45" s="18">
+        <v>2</v>
+      </c>
+      <c r="E45" s="18"/>
+      <c r="F45" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G45" s="19">
+      <c r="G45" s="18">
         <v>13</v>
       </c>
-      <c r="H45" s="19" t="s">
+      <c r="H45" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I45" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J45" s="19" t="s">
+      <c r="I45" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J45" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="21" t="s">
+    <row r="46" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22" t="s">
+      <c r="B46" s="21"/>
+      <c r="C46" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="D46" s="19">
-        <v>2</v>
-      </c>
-      <c r="E46" s="19"/>
-      <c r="F46" s="23" t="s">
+      <c r="D46" s="18">
+        <v>2</v>
+      </c>
+      <c r="E46" s="18"/>
+      <c r="F46" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G46" s="19">
+      <c r="G46" s="18">
         <v>11</v>
       </c>
-      <c r="H46" s="19" t="s">
+      <c r="H46" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I46" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J46" s="19" t="s">
+      <c r="I46" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J46" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="21" t="s">
+    <row r="47" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22" t="s">
+      <c r="B47" s="21"/>
+      <c r="C47" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19">
-        <v>2</v>
-      </c>
-      <c r="F47" s="23" t="s">
+      <c r="D47" s="18"/>
+      <c r="E47" s="18">
+        <v>2</v>
+      </c>
+      <c r="F47" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G47" s="19" t="s">
+      <c r="G47" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="H47" s="19" t="s">
+      <c r="H47" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I47" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J47" s="19" t="s">
+      <c r="I47" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J47" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="21" t="s">
+    <row r="48" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="B48" s="22"/>
-      <c r="C48" s="22" t="s">
+      <c r="B48" s="21"/>
+      <c r="C48" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="D48" s="19">
-        <v>2</v>
-      </c>
-      <c r="E48" s="19"/>
-      <c r="F48" s="23" t="s">
+      <c r="D48" s="18">
+        <v>2</v>
+      </c>
+      <c r="E48" s="18"/>
+      <c r="F48" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G48" s="19">
+      <c r="G48" s="18">
         <v>12</v>
       </c>
-      <c r="H48" s="19" t="s">
+      <c r="H48" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I48" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J48" s="19"/>
-    </row>
-    <row r="49" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="21" t="s">
+      <c r="I48" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J48" s="18"/>
+    </row>
+    <row r="49" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="B49" s="22"/>
-      <c r="C49" s="22" t="s">
+      <c r="B49" s="21"/>
+      <c r="C49" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="D49" s="19">
-        <v>2</v>
-      </c>
-      <c r="E49" s="19"/>
-      <c r="F49" s="23" t="s">
+      <c r="D49" s="18">
+        <v>2</v>
+      </c>
+      <c r="E49" s="18"/>
+      <c r="F49" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G49" s="19">
+      <c r="G49" s="18">
         <v>14</v>
       </c>
-      <c r="H49" s="19" t="s">
+      <c r="H49" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I49" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J49" s="19" t="s">
+      <c r="I49" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J49" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="21" t="s">
+    <row r="50" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="B50" s="22"/>
-      <c r="C50" s="22" t="s">
+      <c r="B50" s="21"/>
+      <c r="C50" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="D50" s="19">
-        <v>2</v>
-      </c>
-      <c r="E50" s="19"/>
-      <c r="F50" s="23" t="s">
+      <c r="D50" s="18">
+        <v>2</v>
+      </c>
+      <c r="E50" s="18"/>
+      <c r="F50" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G50" s="19">
+      <c r="G50" s="18">
         <v>15</v>
       </c>
-      <c r="H50" s="19" t="s">
+      <c r="H50" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I50" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J50" s="19" t="s">
+      <c r="I50" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J50" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="21" t="s">
+    <row r="51" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="B51" s="22"/>
-      <c r="C51" s="22" t="s">
+      <c r="B51" s="21"/>
+      <c r="C51" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="D51" s="19">
-        <v>2</v>
-      </c>
-      <c r="E51" s="19"/>
-      <c r="F51" s="23" t="s">
+      <c r="D51" s="18">
+        <v>2</v>
+      </c>
+      <c r="E51" s="18"/>
+      <c r="F51" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G51" s="19">
+      <c r="G51" s="18">
         <v>13</v>
       </c>
-      <c r="H51" s="19" t="s">
+      <c r="H51" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I51" s="19" t="s">
+      <c r="I51" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J51" s="19" t="s">
+      <c r="J51" s="18" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="21" t="s">
+    <row r="52" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22" t="s">
+      <c r="B52" s="21"/>
+      <c r="C52" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19">
-        <v>2</v>
-      </c>
-      <c r="F52" s="23" t="s">
+      <c r="D52" s="18"/>
+      <c r="E52" s="18">
+        <v>2</v>
+      </c>
+      <c r="F52" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G52" s="19">
+      <c r="G52" s="18">
         <v>12</v>
       </c>
-      <c r="H52" s="19" t="s">
+      <c r="H52" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I52" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J52" s="19" t="s">
+      <c r="I52" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J52" s="18" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="21" t="s">
+    <row r="53" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="B53" s="22"/>
-      <c r="C53" s="22" t="s">
+      <c r="B53" s="21"/>
+      <c r="C53" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19">
-        <v>2</v>
-      </c>
-      <c r="F53" s="23" t="s">
+      <c r="D53" s="18"/>
+      <c r="E53" s="18">
+        <v>2</v>
+      </c>
+      <c r="F53" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G53" s="19">
+      <c r="G53" s="18">
         <v>13</v>
       </c>
-      <c r="H53" s="19" t="s">
+      <c r="H53" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I53" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J53" s="19" t="s">
+      <c r="I53" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J53" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="21" t="s">
+    <row r="54" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="B54" s="22"/>
-      <c r="C54" s="22" t="s">
+      <c r="B54" s="21"/>
+      <c r="C54" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="D54" s="19">
-        <v>2</v>
-      </c>
-      <c r="E54" s="19"/>
-      <c r="F54" s="23" t="s">
+      <c r="D54" s="18">
+        <v>2</v>
+      </c>
+      <c r="E54" s="18"/>
+      <c r="F54" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G54" s="19">
+      <c r="G54" s="18">
         <v>16</v>
       </c>
-      <c r="H54" s="19" t="s">
+      <c r="H54" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I54" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J54" s="19" t="s">
+      <c r="I54" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J54" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="21" t="s">
+    <row r="55" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="B55" s="22"/>
-      <c r="C55" s="22" t="s">
+      <c r="B55" s="21"/>
+      <c r="C55" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="D55" s="19">
-        <v>2</v>
-      </c>
-      <c r="E55" s="19"/>
-      <c r="F55" s="23" t="s">
+      <c r="D55" s="18">
+        <v>2</v>
+      </c>
+      <c r="E55" s="18"/>
+      <c r="F55" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G55" s="19">
+      <c r="G55" s="18">
         <v>17</v>
       </c>
-      <c r="H55" s="19" t="s">
+      <c r="H55" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I55" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J55" s="19" t="s">
+      <c r="I55" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J55" s="18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="21" t="s">
+    <row r="56" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="B56" s="22"/>
-      <c r="C56" s="22" t="s">
+      <c r="B56" s="21"/>
+      <c r="C56" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="D56" s="19">
-        <v>2</v>
-      </c>
-      <c r="E56" s="19"/>
-      <c r="F56" s="23" t="s">
+      <c r="D56" s="18">
+        <v>2</v>
+      </c>
+      <c r="E56" s="18"/>
+      <c r="F56" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G56" s="19">
+      <c r="G56" s="18">
         <v>14</v>
       </c>
-      <c r="H56" s="19" t="s">
+      <c r="H56" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I56" s="19" t="s">
+      <c r="I56" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="J56" s="19" t="s">
+      <c r="J56" s="18" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="21" t="s">
+    <row r="57" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="B57" s="22"/>
-      <c r="C57" s="22" t="s">
+      <c r="B57" s="21"/>
+      <c r="C57" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="D57" s="19">
-        <v>2</v>
-      </c>
-      <c r="E57" s="19"/>
-      <c r="F57" s="23" t="s">
+      <c r="D57" s="18">
+        <v>2</v>
+      </c>
+      <c r="E57" s="18"/>
+      <c r="F57" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G57" s="19">
+      <c r="G57" s="18">
         <v>18</v>
       </c>
-      <c r="H57" s="19" t="s">
+      <c r="H57" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I57" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J57" s="19" t="s">
+      <c r="I57" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J57" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="21" t="s">
+    <row r="58" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="B58" s="22"/>
-      <c r="C58" s="22" t="s">
+      <c r="B58" s="21"/>
+      <c r="C58" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19">
-        <v>2</v>
-      </c>
-      <c r="F58" s="23" t="s">
+      <c r="D58" s="18"/>
+      <c r="E58" s="18">
+        <v>2</v>
+      </c>
+      <c r="F58" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G58" s="19">
+      <c r="G58" s="18">
         <v>14</v>
       </c>
-      <c r="H58" s="19" t="s">
+      <c r="H58" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I58" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J58" s="19" t="s">
+      <c r="I58" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J58" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="21" t="s">
+    <row r="59" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="B59" s="22"/>
-      <c r="C59" s="22" t="s">
+      <c r="B59" s="21"/>
+      <c r="C59" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="D59" s="19">
-        <v>2</v>
-      </c>
-      <c r="E59" s="19"/>
-      <c r="F59" s="23" t="s">
+      <c r="D59" s="18">
+        <v>2</v>
+      </c>
+      <c r="E59" s="18"/>
+      <c r="F59" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G59" s="19">
+      <c r="G59" s="18">
         <v>15</v>
       </c>
-      <c r="H59" s="19" t="s">
+      <c r="H59" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I59" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J59" s="19" t="s">
+      <c r="I59" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J59" s="18" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="21" t="s">
+    <row r="60" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="B60" s="22"/>
-      <c r="C60" s="22" t="s">
+      <c r="B60" s="21"/>
+      <c r="C60" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="D60" s="19">
-        <v>2</v>
-      </c>
-      <c r="E60" s="19"/>
-      <c r="F60" s="23" t="s">
+      <c r="D60" s="18">
+        <v>2</v>
+      </c>
+      <c r="E60" s="18"/>
+      <c r="F60" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G60" s="19">
+      <c r="G60" s="18">
         <v>19</v>
       </c>
-      <c r="H60" s="19" t="s">
+      <c r="H60" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I60" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J60" s="19" t="s">
+      <c r="I60" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J60" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="21" t="s">
+    <row r="61" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="B61" s="22"/>
-      <c r="C61" s="22" t="s">
+      <c r="B61" s="21"/>
+      <c r="C61" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="D61" s="19">
-        <v>2</v>
-      </c>
-      <c r="E61" s="19"/>
-      <c r="F61" s="23" t="s">
+      <c r="D61" s="18">
+        <v>2</v>
+      </c>
+      <c r="E61" s="18"/>
+      <c r="F61" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G61" s="19">
+      <c r="G61" s="18">
         <v>20</v>
       </c>
-      <c r="H61" s="19" t="s">
+      <c r="H61" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I61" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J61" s="19" t="s">
+      <c r="I61" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J61" s="18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="21" t="s">
+    <row r="62" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="B62" s="22"/>
-      <c r="C62" s="22" t="s">
+      <c r="B62" s="21"/>
+      <c r="C62" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="D62" s="19">
-        <v>2</v>
-      </c>
-      <c r="E62" s="19"/>
-      <c r="F62" s="23" t="s">
+      <c r="D62" s="18">
+        <v>2</v>
+      </c>
+      <c r="E62" s="18"/>
+      <c r="F62" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G62" s="19">
+      <c r="G62" s="18">
         <v>16</v>
       </c>
-      <c r="H62" s="19" t="s">
+      <c r="H62" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I62" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J62" s="19" t="s">
+      <c r="I62" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J62" s="18" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="21" t="s">
+    <row r="63" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="B63" s="22"/>
-      <c r="C63" s="22" t="s">
+      <c r="B63" s="21"/>
+      <c r="C63" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="D63" s="19">
-        <v>2</v>
-      </c>
-      <c r="E63" s="19"/>
-      <c r="F63" s="23" t="s">
+      <c r="D63" s="18">
+        <v>2</v>
+      </c>
+      <c r="E63" s="18"/>
+      <c r="F63" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G63" s="19">
+      <c r="G63" s="18">
         <v>21</v>
       </c>
-      <c r="H63" s="19" t="s">
+      <c r="H63" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I63" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J63" s="19" t="s">
+      <c r="I63" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J63" s="18" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="21" t="s">
+    <row r="64" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="B64" s="22"/>
-      <c r="C64" s="22" t="s">
+      <c r="B64" s="21"/>
+      <c r="C64" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19">
-        <v>2</v>
-      </c>
-      <c r="F64" s="23" t="s">
+      <c r="D64" s="18"/>
+      <c r="E64" s="18">
+        <v>2</v>
+      </c>
+      <c r="F64" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G64" s="19">
+      <c r="G64" s="18">
         <v>15</v>
       </c>
-      <c r="H64" s="19" t="s">
+      <c r="H64" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I64" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J64" s="19" t="s">
+      <c r="I64" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J64" s="18" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="21" t="s">
+    <row r="65" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="B65" s="22"/>
-      <c r="C65" s="22" t="s">
+      <c r="B65" s="21"/>
+      <c r="C65" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19">
-        <v>2</v>
-      </c>
-      <c r="F65" s="23" t="s">
+      <c r="D65" s="18"/>
+      <c r="E65" s="18">
+        <v>2</v>
+      </c>
+      <c r="F65" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G65" s="19">
+      <c r="G65" s="18">
         <v>16</v>
       </c>
-      <c r="H65" s="19" t="s">
+      <c r="H65" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I65" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J65" s="19" t="s">
+      <c r="I65" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J65" s="18" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="21" t="s">
+    <row r="66" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="B66" s="22"/>
-      <c r="C66" s="22" t="s">
+      <c r="B66" s="21"/>
+      <c r="C66" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="D66" s="19">
-        <v>2</v>
-      </c>
-      <c r="E66" s="19"/>
-      <c r="F66" s="23" t="s">
+      <c r="D66" s="18">
+        <v>2</v>
+      </c>
+      <c r="E66" s="18"/>
+      <c r="F66" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G66" s="19">
+      <c r="G66" s="18">
         <v>22</v>
       </c>
-      <c r="H66" s="19" t="s">
+      <c r="H66" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I66" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J66" s="19" t="s">
+      <c r="I66" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J66" s="18" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="21" t="s">
+    <row r="67" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="20" t="s">
         <v>169</v>
       </c>
       <c r="B67" s="16">
@@ -3014,231 +2963,71 @@
       <c r="C67" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="D67" s="19"/>
-      <c r="E67" s="19"/>
-      <c r="F67" s="23"/>
-      <c r="G67" s="19"/>
-      <c r="H67" s="20"/>
-      <c r="I67" s="19"/>
-      <c r="J67" s="19"/>
-    </row>
-    <row r="68" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="21" t="s">
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="18"/>
+      <c r="H67" s="19"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+    </row>
+    <row r="68" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="22" t="s">
+      <c r="B68" s="21"/>
+      <c r="C68" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="D68" s="19">
-        <v>2</v>
-      </c>
-      <c r="E68" s="19"/>
-      <c r="F68" s="23" t="s">
+      <c r="D68" s="18">
+        <v>2</v>
+      </c>
+      <c r="E68" s="18"/>
+      <c r="F68" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G68" s="19">
+      <c r="G68" s="18">
         <v>17</v>
       </c>
-      <c r="H68" s="19" t="s">
+      <c r="H68" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I68" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J68" s="19" t="s">
+      <c r="I68" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J68" s="18" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="21" t="s">
+    <row r="69" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="B69" s="22"/>
-      <c r="C69" s="22" t="s">
+      <c r="B69" s="21"/>
+      <c r="C69" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19">
-        <v>2</v>
-      </c>
-      <c r="F69" s="23" t="s">
+      <c r="D69" s="18"/>
+      <c r="E69" s="18">
+        <v>2</v>
+      </c>
+      <c r="F69" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="G69" s="19">
+      <c r="G69" s="18">
         <v>17</v>
       </c>
-      <c r="H69" s="19" t="s">
+      <c r="H69" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I69" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J69" s="19" t="s">
+      <c r="I69" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J69" s="18" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="B70" s="22"/>
-      <c r="C70" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="D70" s="19"/>
-      <c r="E70" s="19">
-        <v>1</v>
-      </c>
-      <c r="F70" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G70" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="H70" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="I70" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J70" s="19" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="B71" s="22"/>
-      <c r="C71" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="D71" s="19">
-        <v>2</v>
-      </c>
-      <c r="E71" s="19"/>
-      <c r="F71" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G71" s="19">
-        <v>23</v>
-      </c>
-      <c r="H71" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="I71" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J71" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="B72" s="22"/>
-      <c r="C72" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="D72" s="19">
-        <v>2</v>
-      </c>
-      <c r="E72" s="19"/>
-      <c r="F72" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G72" s="19">
-        <v>24</v>
-      </c>
-      <c r="H72" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="I72" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J72" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="B73" s="22"/>
-      <c r="C73" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="D73" s="19">
-        <v>2</v>
-      </c>
-      <c r="E73" s="19"/>
-      <c r="F73" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="G73" s="19">
-        <v>25</v>
-      </c>
-      <c r="H73" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="I73" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="J73" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="B74" s="22"/>
-      <c r="C74" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="D74" s="19">
-        <v>1</v>
-      </c>
-      <c r="E74" s="19"/>
-      <c r="F74" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="G74" s="19">
-        <v>18</v>
-      </c>
-      <c r="H74" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="I74" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="J74" s="19" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="B75" s="26"/>
-      <c r="C75" s="26" t="s">
-        <v>190</v>
-      </c>
-      <c r="D75" s="27">
-        <v>85</v>
-      </c>
-      <c r="E75" s="27">
-        <v>35</v>
-      </c>
-      <c r="F75" s="17"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="19"/>
-      <c r="I75" s="19"/>
-      <c r="J75" s="19"/>
-    </row>
-    <row r="76" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F76">
         <f>COUNTIF(F22:F41,"Лабораторна №")</f>
         <v>8</v>
@@ -3246,6 +3035,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="F9:G9"/>
@@ -3262,9 +3054,6 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New changes master (second)
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zerzor13\web-prog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zerzor13\dir_for_git\14_lab\web-prog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1702006-B86D-4632-B388-3C75CF8A9671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B56BF3-1F3F-434D-B3D6-D849B3B73021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="2325" windowWidth="21600" windowHeight="11295" xr2:uid="{5407CB4B-62E8-4971-B1DD-41A867E52758}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5407CB4B-62E8-4971-B1DD-41A867E52758}"/>
   </bookViews>
   <sheets>
     <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
@@ -787,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -860,58 +860,59 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -1228,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AB4ACD-37B1-4AC7-AF77-03DE915FAA9E}">
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1242,18 +1243,18 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="33" t="s">
+      <c r="B1" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="33" t="s">
+      <c r="E1" s="35"/>
+      <c r="F1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="34"/>
+      <c r="G1" s="35"/>
       <c r="H1" s="5" t="s">
         <v>13</v>
       </c>
@@ -1266,16 +1267,16 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="38"/>
+      <c r="G2" s="47"/>
       <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
@@ -1288,16 +1289,16 @@
     </row>
     <row r="3" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="38"/>
+      <c r="G3" s="47"/>
       <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
@@ -1310,14 +1311,14 @@
     </row>
     <row r="4" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="38"/>
+      <c r="G4" s="47"/>
       <c r="H4" s="6" t="s">
         <v>16</v>
       </c>
@@ -1328,14 +1329,14 @@
     </row>
     <row r="5" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="38"/>
+      <c r="G5" s="47"/>
       <c r="H5" s="6" t="s">
         <v>17</v>
       </c>
@@ -1344,14 +1345,14 @@
     </row>
     <row r="6" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37" t="s">
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="38"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="7" t="s">
         <v>12</v>
       </c>
@@ -1360,30 +1361,30 @@
     </row>
     <row r="7" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="37" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="38"/>
+      <c r="G7" s="47"/>
       <c r="H7" s="7"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="32"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="45"/>
       <c r="D8" s="11" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="41"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
@@ -1392,20 +1393,20 @@
       <c r="A9" s="13">
         <v>1</v>
       </c>
-      <c r="B9" s="29">
-        <v>2</v>
-      </c>
-      <c r="C9" s="30"/>
+      <c r="B9" s="42">
+        <v>2</v>
+      </c>
+      <c r="C9" s="43"/>
       <c r="D9" s="14">
         <v>3</v>
       </c>
       <c r="E9" s="14">
         <v>4</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="42">
         <v>5</v>
       </c>
-      <c r="G9" s="30"/>
+      <c r="G9" s="43"/>
       <c r="H9" s="14">
         <v>6</v>
       </c>
@@ -3055,163 +3056,171 @@
       </c>
     </row>
     <row r="70" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="39">
+      <c r="A70" s="25">
         <v>1</v>
       </c>
-      <c r="B70" s="40">
+      <c r="B70" s="26">
         <v>1</v>
       </c>
-      <c r="C70" s="40">
+      <c r="C70" s="26">
         <v>1</v>
       </c>
-      <c r="D70" s="40">
+      <c r="D70" s="26">
         <v>1</v>
       </c>
-      <c r="E70" s="40">
+      <c r="E70" s="26">
         <v>1</v>
       </c>
-      <c r="F70" s="40">
+      <c r="F70" s="26">
         <v>1</v>
       </c>
-      <c r="G70" s="40">
+      <c r="G70" s="26">
         <v>1</v>
       </c>
-      <c r="H70" s="40">
+      <c r="H70" s="26">
         <v>1</v>
       </c>
-      <c r="I70" s="40">
+      <c r="I70" s="26">
         <v>1</v>
       </c>
-      <c r="J70" s="41">
+      <c r="J70" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="42">
-        <v>2</v>
-      </c>
-      <c r="B71" s="43">
-        <v>2</v>
-      </c>
-      <c r="C71" s="43">
-        <v>2</v>
-      </c>
-      <c r="D71" s="43">
-        <v>2</v>
-      </c>
-      <c r="E71" s="43">
-        <v>2</v>
-      </c>
-      <c r="F71" s="43">
-        <v>2</v>
-      </c>
-      <c r="G71" s="43">
-        <v>2</v>
-      </c>
-      <c r="H71" s="43">
-        <v>2</v>
-      </c>
-      <c r="I71" s="43">
-        <v>2</v>
-      </c>
-      <c r="J71" s="44">
+      <c r="A71" s="28">
+        <v>2</v>
+      </c>
+      <c r="B71" s="29">
+        <v>2</v>
+      </c>
+      <c r="C71" s="29">
+        <v>2</v>
+      </c>
+      <c r="D71" s="29">
+        <v>2</v>
+      </c>
+      <c r="E71" s="29">
+        <v>2</v>
+      </c>
+      <c r="F71" s="29">
+        <v>2</v>
+      </c>
+      <c r="G71" s="29">
+        <v>2</v>
+      </c>
+      <c r="H71" s="29">
+        <v>2</v>
+      </c>
+      <c r="I71" s="29">
+        <v>2</v>
+      </c>
+      <c r="J71" s="30">
         <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="42">
+      <c r="A72" s="28">
         <v>3</v>
       </c>
-      <c r="B72" s="43">
+      <c r="B72" s="29">
         <v>3</v>
       </c>
-      <c r="C72" s="43">
+      <c r="C72" s="29">
         <v>3</v>
       </c>
-      <c r="D72" s="43">
+      <c r="D72" s="29">
         <v>3</v>
       </c>
-      <c r="E72" s="43">
+      <c r="E72" s="29">
         <v>3</v>
       </c>
-      <c r="F72" s="43">
+      <c r="F72" s="29">
         <v>3</v>
       </c>
-      <c r="G72" s="43">
+      <c r="G72" s="29">
         <v>3</v>
       </c>
-      <c r="H72" s="43">
+      <c r="H72" s="29">
         <v>3</v>
       </c>
-      <c r="I72" s="43">
+      <c r="I72" s="29">
         <v>3</v>
       </c>
-      <c r="J72" s="44">
+      <c r="J72" s="30">
         <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="42">
+      <c r="A73" s="28">
         <v>4</v>
       </c>
-      <c r="B73" s="43">
+      <c r="B73" s="29">
         <v>4</v>
       </c>
-      <c r="C73" s="43">
+      <c r="C73" s="29">
         <v>4</v>
       </c>
-      <c r="D73" s="43">
+      <c r="D73" s="29">
         <v>4</v>
       </c>
-      <c r="E73" s="43">
+      <c r="E73" s="29">
         <v>4</v>
       </c>
-      <c r="F73" s="43">
+      <c r="F73" s="29">
         <v>4</v>
       </c>
-      <c r="G73" s="43">
+      <c r="G73" s="29">
         <v>4</v>
       </c>
-      <c r="H73" s="43">
+      <c r="H73" s="29">
         <v>4</v>
       </c>
-      <c r="I73" s="43">
+      <c r="I73" s="29">
         <v>4</v>
       </c>
-      <c r="J73" s="44">
+      <c r="J73" s="30">
         <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="20.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="45">
+      <c r="A74" s="31">
         <v>5</v>
       </c>
-      <c r="B74" s="46">
+      <c r="B74" s="32">
         <v>5</v>
       </c>
-      <c r="C74" s="46">
+      <c r="C74" s="32">
         <v>5</v>
       </c>
-      <c r="D74" s="46">
+      <c r="D74" s="32">
         <v>5</v>
       </c>
-      <c r="E74" s="46">
+      <c r="E74" s="32">
         <v>5</v>
       </c>
-      <c r="F74" s="46">
+      <c r="F74" s="32">
         <v>5</v>
       </c>
-      <c r="G74" s="46">
+      <c r="G74" s="32">
         <v>5</v>
       </c>
-      <c r="H74" s="46">
+      <c r="H74" s="32">
         <v>5</v>
       </c>
-      <c r="I74" s="46">
+      <c r="I74" s="32">
         <v>5</v>
       </c>
-      <c r="J74" s="47">
+      <c r="J74" s="33">
         <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="28">
+        <v>1</v>
+      </c>
+      <c r="B75" s="48">
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3222,11 +3231,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="B9:C9"/>
@@ -3241,6 +3245,11 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>